<commit_message>
added diffrent security conditions for 1h and 1m orders; cleaning code; fixed coupe bugs;
</commit_message>
<xml_diff>
--- a/db/bin/real_trade_db_2024-09-11.xlsx
+++ b/db/bin/real_trade_db_2024-09-11.xlsx
@@ -16899,7 +16899,7 @@
         </is>
       </c>
       <c r="D193" s="2" t="n">
-        <v>45546.04770819391</v>
+        <v>45546.04770819444</v>
       </c>
       <c r="E193" t="n">
         <v>591.1</v>
@@ -16981,7 +16981,7 @@
         </is>
       </c>
       <c r="D194" s="2" t="n">
-        <v>45546.06248326154</v>
+        <v>45546.06248326389</v>
       </c>
       <c r="E194" t="n">
         <v>227.83</v>
@@ -17063,7 +17063,7 @@
         </is>
       </c>
       <c r="D195" s="2" t="n">
-        <v>45546.06877688242</v>
+        <v>45546.06877688658</v>
       </c>
       <c r="E195" t="n">
         <v>73.5</v>
@@ -17145,7 +17145,7 @@
         </is>
       </c>
       <c r="D196" s="2" t="n">
-        <v>45546.07164919913</v>
+        <v>45546.07164920139</v>
       </c>
       <c r="E196" t="n">
         <v>362.82</v>
@@ -17227,7 +17227,7 @@
         </is>
       </c>
       <c r="D197" s="2" t="n">
-        <v>45546.07184414212</v>
+        <v>45546.07184414352</v>
       </c>
       <c r="E197" t="n">
         <v>138.61</v>
@@ -17309,7 +17309,7 @@
         </is>
       </c>
       <c r="D198" s="2" t="n">
-        <v>45546.07240959213</v>
+        <v>45546.0724095949</v>
       </c>
       <c r="E198" t="n">
         <v>85.49930000000001</v>
@@ -17405,7 +17405,7 @@
         </is>
       </c>
       <c r="D199" s="2" t="n">
-        <v>45546.10861399129</v>
+        <v>45546.10861399306</v>
       </c>
       <c r="E199" t="n">
         <v>349.73</v>
@@ -17487,7 +17487,7 @@
         </is>
       </c>
       <c r="D200" s="2" t="n">
-        <v>45546.10902002258</v>
+        <v>45546.10902002315</v>
       </c>
       <c r="E200" t="n">
         <v>90.43000000000001</v>
@@ -17569,7 +17569,7 @@
         </is>
       </c>
       <c r="D201" s="2" t="n">
-        <v>45546.13186334349</v>
+        <v>45546.1318633449</v>
       </c>
       <c r="E201" t="n">
         <v>591.1</v>
@@ -17651,7 +17651,7 @@
         </is>
       </c>
       <c r="D202" s="2" t="n">
-        <v>45546.13967005927</v>
+        <v>45546.13967005787</v>
       </c>
       <c r="E202" t="n">
         <v>194.98</v>
@@ -17733,7 +17733,7 @@
         </is>
       </c>
       <c r="D203" s="2" t="n">
-        <v>45546.14184971542</v>
+        <v>45546.14184971065</v>
       </c>
       <c r="E203" t="n">
         <v>363.52</v>
@@ -17815,7 +17815,7 @@
         </is>
       </c>
       <c r="D204" s="2" t="n">
-        <v>45546.14424799271</v>
+        <v>45546.14424799768</v>
       </c>
       <c r="E204" t="n">
         <v>288.98</v>
@@ -17897,7 +17897,7 @@
         </is>
       </c>
       <c r="D205" s="2" t="n">
-        <v>45546.14458235825</v>
+        <v>45546.14458236111</v>
       </c>
       <c r="E205" t="n">
         <v>114.54</v>
@@ -17979,7 +17979,7 @@
         </is>
       </c>
       <c r="D206" s="2" t="n">
-        <v>45546.14874744727</v>
+        <v>45546.14874744213</v>
       </c>
       <c r="E206" t="n">
         <v>53.92</v>
@@ -18061,7 +18061,7 @@
         </is>
       </c>
       <c r="D207" s="2" t="n">
-        <v>45546.14942623025</v>
+        <v>45546.14942622685</v>
       </c>
       <c r="E207" t="n">
         <v>91.26000000000001</v>
@@ -18143,7 +18143,7 @@
         </is>
       </c>
       <c r="D208" s="2" t="n">
-        <v>45546.16101638086</v>
+        <v>45546.16101637731</v>
       </c>
       <c r="E208" t="n">
         <v>364.06</v>
@@ -18225,7 +18225,7 @@
         </is>
       </c>
       <c r="D209" s="2" t="n">
-        <v>45546.16148011265</v>
+        <v>45546.16148011574</v>
       </c>
       <c r="E209" t="n">
         <v>44.1</v>
@@ -18307,7 +18307,7 @@
         </is>
       </c>
       <c r="D210" s="2" t="n">
-        <v>45546.16181439695</v>
+        <v>45546.16181439815</v>
       </c>
       <c r="E210" t="n">
         <v>201.73</v>
@@ -18389,7 +18389,7 @@
         </is>
       </c>
       <c r="D211" s="2" t="n">
-        <v>45546.16339168209</v>
+        <v>45546.16339167824</v>
       </c>
       <c r="E211" t="n">
         <v>56.27</v>
@@ -18471,7 +18471,7 @@
         </is>
       </c>
       <c r="D212" s="2" t="n">
-        <v>45546.16405353545</v>
+        <v>45546.16405353009</v>
       </c>
       <c r="E212" t="n">
         <v>39.03</v>
@@ -18553,7 +18553,7 @@
         </is>
       </c>
       <c r="D213" s="2" t="n">
-        <v>45546.16799073493</v>
+        <v>45546.16799072917</v>
       </c>
       <c r="E213" t="n">
         <v>350.52</v>
@@ -18635,7 +18635,7 @@
         </is>
       </c>
       <c r="D214" s="2" t="n">
-        <v>45546.16820098869</v>
+        <v>45546.1682009838</v>
       </c>
       <c r="E214" t="n">
         <v>235.05</v>
@@ -18717,7 +18717,7 @@
         </is>
       </c>
       <c r="D215" s="2" t="n">
-        <v>45546.169891267</v>
+        <v>45546.16989126158</v>
       </c>
       <c r="E215" t="n">
         <v>201.73</v>
@@ -18799,7 +18799,7 @@
         </is>
       </c>
       <c r="D216" s="2" t="n">
-        <v>45546.17797475229</v>
+        <v>45546.17797475695</v>
       </c>
       <c r="E216" t="n">
         <v>50.92</v>
@@ -18881,7 +18881,7 @@
         </is>
       </c>
       <c r="D217" s="2" t="n">
-        <v>45546.17831177705</v>
+        <v>45546.17831178241</v>
       </c>
       <c r="E217" t="n">
         <v>75.02</v>
@@ -18963,7 +18963,7 @@
         </is>
       </c>
       <c r="D218" s="2" t="n">
-        <v>45546.17921527202</v>
+        <v>45546.17921527778</v>
       </c>
       <c r="E218" t="n">
         <v>320.86</v>
@@ -19045,7 +19045,7 @@
         </is>
       </c>
       <c r="D219" s="2" t="n">
-        <v>45546.19469051333</v>
+        <v>45546.19469050926</v>
       </c>
       <c r="E219" t="n">
         <v>275.24</v>
@@ -19127,7 +19127,7 @@
         </is>
       </c>
       <c r="D220" s="2" t="n">
-        <v>45546.19503070891</v>
+        <v>45546.19503070602</v>
       </c>
       <c r="E220" t="n">
         <v>76.2</v>
@@ -19209,7 +19209,7 @@
         </is>
       </c>
       <c r="D221" s="2" t="n">
-        <v>45546.19921304984</v>
+        <v>45546.19921305556</v>
       </c>
       <c r="E221" t="n">
         <v>323.13</v>
@@ -19291,7 +19291,7 @@
         </is>
       </c>
       <c r="D222" s="2" t="n">
-        <v>45546.20173494409</v>
+        <v>45546.20173494213</v>
       </c>
       <c r="E222" t="n">
         <v>53.92</v>
@@ -19373,7 +19373,7 @@
         </is>
       </c>
       <c r="D223" s="2" t="n">
-        <v>45546.21039305161</v>
+        <v>45546.21039305555</v>
       </c>
       <c r="E223" t="n">
         <v>148.7</v>
@@ -19455,7 +19455,7 @@
         </is>
       </c>
       <c r="D224" s="2" t="n">
-        <v>45546.21262778415</v>
+        <v>45546.21262778935</v>
       </c>
       <c r="E224" t="n">
         <v>73.94</v>
@@ -19537,7 +19537,7 @@
         </is>
       </c>
       <c r="D225" s="2" t="n">
-        <v>45546.21365040055</v>
+        <v>45546.21365040509</v>
       </c>
       <c r="E225" t="n">
         <v>161</v>
@@ -19619,7 +19619,7 @@
         </is>
       </c>
       <c r="D226" s="2" t="n">
-        <v>45546.21535731851</v>
+        <v>45546.21535731482</v>
       </c>
       <c r="E226" t="n">
         <v>91.48</v>
@@ -19701,7 +19701,7 @@
         </is>
       </c>
       <c r="D227" s="2" t="n">
-        <v>45546.22435662566</v>
+        <v>45546.22435662037</v>
       </c>
       <c r="E227" t="n">
         <v>77.15000000000001</v>
@@ -19783,7 +19783,7 @@
         </is>
       </c>
       <c r="D228" s="2" t="n">
-        <v>45546.22519991434</v>
+        <v>45546.22519991898</v>
       </c>
       <c r="E228" t="n">
         <v>460.1</v>
@@ -19865,7 +19865,7 @@
         </is>
       </c>
       <c r="D229" s="2" t="n">
-        <v>45546.22560200509</v>
+        <v>45546.22560200231</v>
       </c>
       <c r="E229" t="n">
         <v>250.26</v>
@@ -19947,7 +19947,7 @@
         </is>
       </c>
       <c r="D230" s="2" t="n">
-        <v>45546.23101879149</v>
+        <v>45546.23101879629</v>
       </c>
       <c r="E230" t="n">
         <v>320.86</v>
@@ -20029,7 +20029,7 @@
         </is>
       </c>
       <c r="D231" s="2" t="n">
-        <v>45546.23505663957</v>
+        <v>45546.23505664352</v>
       </c>
       <c r="E231" t="n">
         <v>275.59</v>
@@ -20111,7 +20111,7 @@
         </is>
       </c>
       <c r="D232" s="2" t="n">
-        <v>45546.23934447494</v>
+        <v>45546.23934447917</v>
       </c>
       <c r="E232" t="n">
         <v>364.17</v>
@@ -20193,7 +20193,7 @@
         </is>
       </c>
       <c r="D233" s="2" t="n">
-        <v>45546.23975686911</v>
+        <v>45546.23975686343</v>
       </c>
       <c r="E233" t="n">
         <v>558.08</v>
@@ -20275,7 +20275,7 @@
         </is>
       </c>
       <c r="D234" s="2" t="n">
-        <v>45546.24124082045</v>
+        <v>45546.24124082176</v>
       </c>
       <c r="E234" t="n">
         <v>669.95</v>
@@ -20357,7 +20357,7 @@
         </is>
       </c>
       <c r="D235" s="2" t="n">
-        <v>45546.24229875412</v>
+        <v>45546.24229875</v>
       </c>
       <c r="E235" t="n">
         <v>89.15000000000001</v>
@@ -20439,7 +20439,7 @@
         </is>
       </c>
       <c r="D236" s="2" t="n">
-        <v>45546.24978713758</v>
+        <v>45546.24978714121</v>
       </c>
       <c r="E236" t="n">
         <v>320.86</v>

</xml_diff>